<commit_message>
fill arrayLenght before each array
</commit_message>
<xml_diff>
--- a/память.xlsx
+++ b/память.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045E94C9-2F29-43CD-B94D-014EBF32FFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9768D3CA-ED1D-4729-8AC0-3A3BE503A795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10995" yWindow="1800" windowWidth="11250" windowHeight="12630" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,6 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -383,7 +384,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -717,14 +717,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1275,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1286,29 +1286,30 @@
     <col min="3" max="6" width="6.625" customWidth="1"/>
     <col min="7" max="7" width="6.375" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="2:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
@@ -1366,7 +1367,7 @@
         <f>IF(F3&gt;0,F3/$H$2,"")</f>
         <v>0.7412109375</v>
       </c>
-      <c r="K3" s="26"/>
+      <c r="K3" s="21"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="19"/>
@@ -1394,8 +1395,8 @@
         <f>IF(F4&gt;0,F4/$H$2,"")</f>
         <v/>
       </c>
-      <c r="K4" s="26">
-        <f t="shared" ref="K3:K13" si="0">G3-G4</f>
+      <c r="K4" s="21">
+        <f t="shared" ref="K3:K15" si="0">IF(AND(G4 &gt; 0,G3 &gt; 0), G3-G4, "")</f>
         <v>2.6041666666666297E-3</v>
       </c>
     </row>
@@ -1425,7 +1426,7 @@
         <f t="shared" ref="J5:J28" si="4">IF(F5&gt;0,F5/$H$2,"")</f>
         <v/>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="21">
         <f t="shared" si="0"/>
         <v>-7.6822916666666741E-3</v>
       </c>
@@ -1462,7 +1463,7 @@
         <f t="shared" si="4"/>
         <v>0.63525390625</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="21">
         <f t="shared" si="0"/>
         <v>7.7473958333333925E-3</v>
       </c>
@@ -1495,7 +1496,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="21">
         <f t="shared" si="0"/>
         <v>-6.9661458333333259E-3</v>
       </c>
@@ -1526,7 +1527,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="21">
         <f t="shared" si="0"/>
         <v>-1.5625000000000222E-3</v>
       </c>
@@ -1561,7 +1562,7 @@
         <f t="shared" si="4"/>
         <v>0.64453125</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="21">
         <f t="shared" si="0"/>
         <v>-9.765625E-3</v>
       </c>
@@ -1592,7 +1593,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="21">
         <f t="shared" si="0"/>
         <v>2.5390625000000222E-3</v>
       </c>
@@ -1623,7 +1624,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="21">
         <f t="shared" si="0"/>
         <v>-5.4036458333333037E-3</v>
       </c>
@@ -1654,7 +1655,7 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="21">
         <f t="shared" si="0"/>
         <v>5.2083333333330373E-4</v>
       </c>
@@ -1689,7 +1690,7 @@
         <f t="shared" si="4"/>
         <v>0.24072265625</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="21">
         <f t="shared" si="0"/>
         <v>1.6276041666666297E-3</v>
       </c>
@@ -1720,24 +1721,28 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K14" s="26">
-        <f>G13-G14</f>
+      <c r="K14" s="21">
+        <f t="shared" si="0"/>
         <v>4.1796875000000067E-2</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="7"/>
+      <c r="C15" s="16">
+        <v>25846</v>
+      </c>
+      <c r="D15" s="7">
+        <v>915</v>
+      </c>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H15" s="8" t="str">
+      <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>0.8413411458333333</v>
+      </c>
+      <c r="H15" s="8">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.44677734375</v>
       </c>
       <c r="I15" s="4" t="str">
         <f t="shared" si="3"/>
@@ -1746,6 +1751,10 @@
       <c r="J15" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
+      </c>
+      <c r="K15" s="21">
+        <f t="shared" si="0"/>
+        <v>-5.5989583333333481E-3</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.2">
@@ -1754,14 +1763,8 @@
       <c r="D16" s="7"/>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H16" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1770,21 +1773,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="21" t="str">
+        <f>IF(AND(G16 &gt; 0,G15 &gt; 0), G15-G16, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="19"/>
       <c r="C17" s="16"/>
       <c r="D17" s="7"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H17" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1793,21 +1794,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="21" t="str">
+        <f t="shared" ref="K17:K28" si="5">IF(AND(G17 &gt; 0,G16 &gt; 0), G16-G17, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="19"/>
       <c r="C18" s="16"/>
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H18" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1816,21 +1815,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="19"/>
       <c r="C19" s="16"/>
       <c r="D19" s="7"/>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H19" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1839,21 +1836,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="19"/>
       <c r="C20" s="16"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H20" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1862,21 +1857,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="19"/>
       <c r="C21" s="16"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H21" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1885,21 +1878,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="19"/>
       <c r="C22" s="16"/>
       <c r="D22" s="7"/>
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H22" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1908,21 +1899,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="19"/>
       <c r="C23" s="16"/>
       <c r="D23" s="7"/>
       <c r="E23" s="6"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H23" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1931,21 +1920,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="19"/>
       <c r="C24" s="16"/>
       <c r="D24" s="7"/>
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H24" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1954,21 +1941,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="19"/>
       <c r="C25" s="16"/>
       <c r="D25" s="7"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H25" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1977,21 +1962,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="19"/>
       <c r="C26" s="16"/>
       <c r="D26" s="7"/>
       <c r="E26" s="6"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H26" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2000,21 +1983,19 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="19"/>
       <c r="C27" s="16"/>
       <c r="D27" s="7"/>
       <c r="E27" s="6"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H27" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="4" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2023,27 +2004,29 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="20"/>
       <c r="C28" s="17"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="11" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H28" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="11" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J28" s="12" t="str">
         <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K28" s="21" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>

</xml_diff>